<commit_message>
Entrega 9 - End update old projects
</commit_message>
<xml_diff>
--- a/P0001/09_FICHAS/N3-FD-General.xlsx
+++ b/P0001/09_FICHAS/N3-FD-General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\S3_Buckets\foa-prod-comp-fenomenologico-bucket\foa_puj_curada\P0001\09_FICHAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejaverianaedu-my.sharepoint.com/personal/crivera_javeriana_edu_co/Documents/Mojana control de archivos/REV_FICHAS/FICHAS/P0001/09_FICHAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{E747C491-3135-4E1F-A63F-A4E4C810BC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D887F7-B70B-4133-A0F6-930C07374691}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{E747C491-3135-4E1F-A63F-A4E4C810BC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF7ADF1-2B18-454B-9C01-ED45CAD33646}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <t>Mapa</t>
   </si>
   <si>
-    <t>pdf y png</t>
+    <t>pdf</t>
   </si>
   <si>
     <t>NA</t>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,25 +218,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -521,28 +510,30 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="36.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="36.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,16 +546,16 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -585,14 +576,14 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="47.25" customHeight="1">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -605,16 +596,16 @@
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="1">
         <v>2021</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -635,14 +626,14 @@
       <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="47.25" customHeight="1">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -655,16 +646,16 @@
       <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1">
         <v>2021</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -685,10 +676,10 @@
       <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>